<commit_message>
Texture not visible but at least no crash
</commit_message>
<xml_diff>
--- a/WorkLogDominik.xlsx
+++ b/WorkLogDominik.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\FH\Sem_5\FH_BIF5_CGRMR_OpenGL-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193F88C5-48C1-4204-BE99-88BF5403EA86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74993E47-B0B6-46CE-AF12-46BEF6C0E44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Kini</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>30min Pause</t>
+  </si>
+  <si>
+    <t>Texture Loading</t>
   </si>
 </sst>
 </file>
@@ -387,10 +390,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L10"/>
+  <dimension ref="B1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C3" sqref="C3:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -546,6 +549,20 @@
         <v>0.8125</v>
       </c>
     </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11" s="2">
+        <v>45679</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.83333333333333337</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>